<commit_message>
Updated PARduino.ino to run on arduino 1.0.5 IDE
</commit_message>
<xml_diff>
--- a/PARduino Bill of Materials.xlsx
+++ b/PARduino Bill of Materials.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>Description</t>
   </si>
@@ -101,9 +100,6 @@
     <t>NE = no enclosure</t>
   </si>
   <si>
-    <t>https://www.batchpcb.com/pcbs/106407</t>
-  </si>
-  <si>
     <t>https://www.sparkfun.com/products/8084</t>
   </si>
   <si>
@@ -134,9 +130,6 @@
     <t>tools</t>
   </si>
   <si>
-    <t>FTDI Basic</t>
-  </si>
-  <si>
     <t>microSD to SD Memory Card Adapter</t>
   </si>
   <si>
@@ -158,9 +151,6 @@
     <t>standoffs and screws</t>
   </si>
   <si>
-    <t>36 inch strap with buckle</t>
-  </si>
-  <si>
     <t>Wire snips</t>
   </si>
   <si>
@@ -177,6 +167,18 @@
   </si>
   <si>
     <t>enclosure (picked up at Bed Bath and Beyond)</t>
+  </si>
+  <si>
+    <t>approx</t>
+  </si>
+  <si>
+    <t>http://www.rei.com/product/848429/redpoint-34-webbing-straps-with-side-release-buckles-package-of-2</t>
+  </si>
+  <si>
+    <t>40 inch strap with buckle</t>
+  </si>
+  <si>
+    <t>FTDI Basic to load program onto the microcontroller</t>
   </si>
 </sst>
 </file>
@@ -575,7 +577,7 @@
   <dimension ref="A2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -595,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -689,7 +691,9 @@
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="10">
+        <v>500</v>
+      </c>
       <c r="D6" s="4">
         <v>1</v>
       </c>
@@ -711,7 +715,9 @@
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="10">
+        <v>150</v>
+      </c>
       <c r="D7" s="4">
         <v>1</v>
       </c>
@@ -736,7 +742,9 @@
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="10">
+        <v>25</v>
+      </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
@@ -744,10 +752,10 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -767,9 +775,7 @@
       <c r="E9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>27</v>
-      </c>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="4">
@@ -789,10 +795,10 @@
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -813,10 +819,10 @@
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -825,13 +831,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="10">
         <v>2.95</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -840,9 +846,11 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="10"/>
+        <v>45</v>
+      </c>
+      <c r="C13" s="10">
+        <v>2</v>
+      </c>
       <c r="D13" s="4">
         <v>2</v>
       </c>
@@ -854,7 +862,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="C14" s="10">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -863,10 +877,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>52</v>
+      </c>
+      <c r="C15" s="10">
+        <v>7</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -874,7 +894,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C16">
         <v>7.99</v>
@@ -886,20 +906,23 @@
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" t="s">
-        <v>38</v>
+        <v>53</v>
+      </c>
+      <c r="C19">
+        <v>14.95</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -907,7 +930,7 @@
     </row>
     <row r="20" spans="2:7">
       <c r="B20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20">
         <v>3.49</v>
@@ -916,38 +939,38 @@
         <v>1</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="2:7">
       <c r="B21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C23">
         <v>16.95</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="2:7">
       <c r="B24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="2:7">
       <c r="B25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -957,14 +980,14 @@
     <hyperlink ref="G5" r:id="rId3"/>
     <hyperlink ref="G6" r:id="rId4"/>
     <hyperlink ref="G7" r:id="rId5"/>
-    <hyperlink ref="G9" r:id="rId6"/>
-    <hyperlink ref="G10" r:id="rId7"/>
-    <hyperlink ref="G12" r:id="rId8"/>
-    <hyperlink ref="G11" r:id="rId9"/>
-    <hyperlink ref="G8" r:id="rId10"/>
-    <hyperlink ref="G20" r:id="rId11"/>
-    <hyperlink ref="G23" r:id="rId12"/>
-    <hyperlink ref="G16" r:id="rId13"/>
+    <hyperlink ref="G10" r:id="rId6"/>
+    <hyperlink ref="G12" r:id="rId7"/>
+    <hyperlink ref="G11" r:id="rId8"/>
+    <hyperlink ref="G8" r:id="rId9"/>
+    <hyperlink ref="G20" r:id="rId10"/>
+    <hyperlink ref="G23" r:id="rId11"/>
+    <hyperlink ref="G16" r:id="rId12"/>
+    <hyperlink ref="G15" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId14"/>

</xml_diff>